<commit_message>
Added new weapon type: Guns.
- Added class Skills for Dancers.
- Adding guns to the back end logic.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="208">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -247,7 +247,16 @@
     <t xml:space="preserve">Hell Forged</t>
   </si>
   <si>
-    <t xml:space="preserve">Forged in the depths of hell it's self, it is rumoured that this sword was used by Satan him self to slay thousands of legions of Angelic beings when they invaded Hell.</t>
+    <t xml:space="preserve">Forged in the depths of hell it's self, it is rumored that this sword was used by Satan him self to slay thousands of legions of Angelic beings when they invaded Hell.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magma Based Blaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forged in Magma, this gun blasts out the flames of Hell.</t>
   </si>
   <si>
     <t xml:space="preserve">Hell Forged Staff of Doom</t>
@@ -301,7 +310,7 @@
     <t xml:space="preserve">ring</t>
   </si>
   <si>
-    <t xml:space="preserve">A dream in hell? A single dream of Heaven t's self plagues the minds of the demonic entities that stalk you.</t>
+    <t xml:space="preserve">A dream in hell? A single dream of Heaven, it’s self plagues the minds of the demonic entities that stalk you.</t>
   </si>
   <si>
     <t xml:space="preserve">Hell Forged Chain Leggings</t>
@@ -346,7 +355,7 @@
     <t xml:space="preserve">feet</t>
   </si>
   <si>
-    <t xml:space="preserve">Plate boots created in the magma of the erupting volcanos of hell.</t>
+    <t xml:space="preserve">Plate boots created in the magma of the erupting volcano s of hell.</t>
   </si>
   <si>
     <t xml:space="preserve">Hell Forged Bow of Demonic Dreams</t>
@@ -376,6 +385,12 @@
     <t xml:space="preserve">Pull the trigger, blast them away. Watch the enemy fall to the ground and slowly bleed out</t>
   </si>
   <si>
+    <t xml:space="preserve">Oceans Drowned Bullet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A gun that was found at the bottom of the ocean, drowning in the memories of the past</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oceanic Mages Stave of the Waters</t>
   </si>
   <si>
@@ -454,6 +469,12 @@
     <t xml:space="preserve">An axe created in the mind of The Creator. One full of the most deprave thoughts. it will haunt your dreams</t>
   </si>
   <si>
+    <t xml:space="preserve">Purgatory Smith’s Shotgun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shotgun used by the smith him self.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Purgatory Chains Staff of Life</t>
   </si>
   <si>
@@ -539,6 +560,12 @@
   </si>
   <si>
     <t xml:space="preserve">Created from ice, when this whip cracks the air will freeze the enemy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Queens Frozen Pistol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A gun created of corrupted memories and covered in blood.</t>
   </si>
   <si>
     <t xml:space="preserve">Ice Shard Stave</t>
@@ -897,10 +924,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT56"/>
+  <dimension ref="A1:BT60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="47:47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1307,7 +1334,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>76</v>
@@ -1339,7 +1366,10 @@
       <c r="Q3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="X3" s="1" t="n">
+      <c r="T3" s="1" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="V3" s="1" t="n">
         <v>0.45</v>
       </c>
       <c r="Y3" s="1" t="n">
@@ -1417,7 +1447,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>79</v>
@@ -1431,8 +1461,8 @@
       <c r="G4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="1" t="n">
-        <v>7000</v>
+      <c r="I4" s="1" t="n">
+        <v>2000</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>150000000000</v>
@@ -1446,14 +1476,17 @@
       <c r="O4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="W4" s="1" t="n">
+      <c r="Q4" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X4" s="1" t="n">
         <v>0.45</v>
       </c>
       <c r="Y4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z4" s="1" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="1" t="n">
         <v>1</v>
@@ -1485,11 +1518,8 @@
       <c r="AY4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AZ4" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BA4" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB4" s="1" t="n">
         <v>0</v>
@@ -1527,7 +1557,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>82</v>
@@ -1541,7 +1571,7 @@
       <c r="G5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>7000</v>
       </c>
       <c r="L5" s="1" t="n">
@@ -1556,7 +1586,7 @@
       <c r="O5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X5" s="1" t="n">
+      <c r="W5" s="1" t="n">
         <v>0.45</v>
       </c>
       <c r="Y5" s="1" t="n">
@@ -1595,8 +1625,11 @@
       <c r="AY5" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ5" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB5" s="1" t="n">
         <v>0</v>
@@ -1634,7 +1667,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>225</v>
+        <v>688</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>85</v>
@@ -1648,11 +1681,8 @@
       <c r="G6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>463429</v>
+      <c r="I6" s="1" t="n">
+        <v>7000</v>
       </c>
       <c r="L6" s="1" t="n">
         <v>150000000000</v>
@@ -1666,29 +1696,14 @@
       <c r="O6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S6" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="T6" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="U6" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="V6" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="W6" s="1" t="n">
-        <v>0.3</v>
-      </c>
       <c r="X6" s="1" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="Y6" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="1" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="AC6" s="1" t="n">
         <v>1</v>
@@ -1759,7 +1774,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>266</v>
+        <v>225</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>88</v>
@@ -1773,8 +1788,11 @@
       <c r="G7" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="K7" s="1" t="n">
-        <v>693774</v>
+        <v>463429</v>
       </c>
       <c r="L7" s="1" t="n">
         <v>150000000000</v>
@@ -1791,14 +1809,26 @@
       <c r="S7" s="1" t="n">
         <v>0.05</v>
       </c>
+      <c r="T7" s="1" t="n">
+        <v>0.3</v>
+      </c>
       <c r="U7" s="1" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="Y7" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="Z7" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AC7" s="1" t="n">
         <v>1</v>
@@ -1869,7 +1899,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>677</v>
+        <v>266</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>91</v>
@@ -1883,8 +1913,8 @@
       <c r="G8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="1" t="n">
-        <v>500</v>
+      <c r="K8" s="1" t="n">
+        <v>693774</v>
       </c>
       <c r="L8" s="1" t="n">
         <v>150000000000</v>
@@ -1898,15 +1928,12 @@
       <c r="O8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" s="1" t="n">
+      <c r="S8" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="U8" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="R8" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="S8" s="1" t="n">
-        <v>0.6</v>
-      </c>
       <c r="Y8" s="1" t="n">
         <v>0</v>
       </c>
@@ -1947,16 +1974,16 @@
         <v>0</v>
       </c>
       <c r="BB8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE8" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF8" s="1" t="n">
         <v>0</v>
@@ -1982,7 +2009,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>310</v>
+        <v>677</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>94</v>
@@ -1996,11 +2023,8 @@
       <c r="G9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="1" t="n">
-        <v>465129</v>
+      <c r="I9" s="1" t="n">
+        <v>500</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>150000000000</v>
@@ -2014,29 +2038,20 @@
       <c r="O9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q9" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>0.6</v>
+      </c>
       <c r="S9" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="T9" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="U9" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="V9" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="W9" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="X9" s="1" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="Y9" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="1" t="n">
         <v>1</v>
@@ -2072,16 +2087,16 @@
         <v>0</v>
       </c>
       <c r="BB9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE9" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF9" s="1" t="n">
         <v>0</v>
@@ -2107,7 +2122,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>97</v>
@@ -2125,7 +2140,7 @@
         <v>98</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>463429</v>
+        <v>465129</v>
       </c>
       <c r="L10" s="1" t="n">
         <v>150000000000</v>
@@ -2232,7 +2247,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>692</v>
+        <v>352</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>100</v>
@@ -2246,8 +2261,11 @@
       <c r="G11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="1" t="n">
-        <v>2000</v>
+      <c r="H11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>463429</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>150000000000</v>
@@ -2261,17 +2279,29 @@
       <c r="O11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" s="1" t="n">
-        <v>0.1</v>
+      <c r="S11" s="1" t="n">
+        <v>0.05</v>
       </c>
       <c r="T11" s="1" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="W11" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="X11" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="Y11" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="Z11" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AC11" s="1" t="n">
         <v>1</v>
@@ -2342,7 +2372,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>396</v>
+        <v>692</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>103</v>
@@ -2356,11 +2386,8 @@
       <c r="G12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" s="1" t="n">
-        <v>465129</v>
+      <c r="I12" s="1" t="n">
+        <v>2000</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>150000000000</v>
@@ -2374,29 +2401,17 @@
       <c r="O12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S12" s="1" t="n">
-        <v>0.05</v>
+      <c r="Q12" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="T12" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="U12" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="V12" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="W12" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="X12" s="1" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="Y12" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="1" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="1" t="n">
         <v>1</v>
@@ -2467,7 +2482,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>106</v>
@@ -2485,7 +2500,7 @@
         <v>107</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>461556</v>
+        <v>465129</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>150000000000</v>
@@ -2592,7 +2607,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>695</v>
+        <v>436</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>109</v>
@@ -2606,8 +2621,11 @@
       <c r="G14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="1" t="n">
-        <v>2000</v>
+      <c r="H14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>461556</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>150000000000</v>
@@ -2621,17 +2639,29 @@
       <c r="O14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" s="1" t="n">
-        <v>0.1</v>
+      <c r="S14" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="T14" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="U14" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
+      </c>
+      <c r="W14" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="X14" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="Y14" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="Z14" s="1" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AC14" s="1" t="n">
         <v>1</v>
@@ -2702,7 +2732,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>484</v>
+        <v>695</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>112</v>
@@ -2716,11 +2746,8 @@
       <c r="G15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="1" t="n">
-        <v>936190</v>
+      <c r="I15" s="1" t="n">
+        <v>2000</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>150000000000</v>
@@ -2734,29 +2761,17 @@
       <c r="O15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S15" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="T15" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="U15" s="1" t="n">
-        <v>0.6</v>
+      <c r="Q15" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="W15" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="X15" s="1" t="n">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="Y15" s="1" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="1" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="1" t="n">
         <v>1</v>
@@ -2827,43 +2842,61 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>679</v>
+        <v>484</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="1" t="n">
-        <v>5000</v>
+      <c r="H16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>936190</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>1000000000</v>
+        <v>150000000000</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>1000</v>
       </c>
       <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" s="1" t="n">
-        <v>0.3</v>
+      <c r="S16" s="1" t="n">
+        <v>0.05</v>
       </c>
       <c r="T16" s="1" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
+      </c>
+      <c r="U16" s="1" t="n">
+        <v>0.6</v>
       </c>
       <c r="V16" s="1" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
+      </c>
+      <c r="W16" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="X16" s="1" t="n">
+        <v>0.6</v>
       </c>
       <c r="Y16" s="1" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="Z16" s="1" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AC16" s="1" t="n">
         <v>1</v>
@@ -2917,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="BM16" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN16" s="1" t="n">
         <v>0</v>
@@ -2934,19 +2967,19 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I17" s="1" t="n">
         <v>5000</v>
@@ -2960,7 +2993,10 @@
       <c r="Q17" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="X17" s="1" t="n">
+      <c r="T17" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V17" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y17" s="1" t="n">
@@ -3038,22 +3074,22 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>1000000</v>
+        <v>5000</v>
       </c>
       <c r="L18" s="1" t="n">
         <v>1000000000</v>
@@ -3062,16 +3098,19 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="X18" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T18" s="1" t="n">
         <v>0.7</v>
       </c>
+      <c r="V18" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="Y18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z18" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="1" t="n">
         <v>1</v>
@@ -3142,25 +3181,22 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>213</v>
+        <v>682</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="1" t="n">
-        <v>600000</v>
+        <v>124</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L19" s="1" t="n">
         <v>1000000000</v>
@@ -3168,29 +3204,17 @@
       <c r="O19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S19" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T19" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="U19" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="V19" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="W19" s="1" t="n">
-        <v>0.7</v>
+      <c r="Q19" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="X19" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y19" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="1" t="n">
         <v>1</v>
@@ -3261,21 +3285,21 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>258</v>
+        <v>687</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K20" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="I20" s="1" t="n">
         <v>1000000</v>
       </c>
       <c r="L20" s="1" t="n">
@@ -3284,17 +3308,17 @@
       <c r="O20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S20" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="U20" s="1" t="n">
-        <v>0.8</v>
+      <c r="Q20" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="X20" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z20" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC20" s="1" t="n">
         <v>1</v>
@@ -3365,43 +3389,55 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>690</v>
+        <v>213</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>5000</v>
+        <v>128</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="O21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="R21" s="1" t="n">
+      <c r="S21" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T21" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="S21" s="1" t="n">
-        <v>0.75</v>
+      <c r="U21" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V21" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W21" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="X21" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y21" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Z21" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC21" s="1" t="n">
         <v>1</v>
@@ -3437,16 +3473,16 @@
         <v>0</v>
       </c>
       <c r="BB21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF21" s="1" t="n">
         <v>0</v>
@@ -3472,25 +3508,22 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="K22" s="1" t="n">
-        <v>600000</v>
+        <v>1000000</v>
       </c>
       <c r="L22" s="1" t="n">
         <v>1000000000</v>
@@ -3501,26 +3534,14 @@
       <c r="S22" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="T22" s="1" t="n">
-        <v>0.7</v>
-      </c>
       <c r="U22" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="V22" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="W22" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="X22" s="1" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="Y22" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z22" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC22" s="1" t="n">
         <v>1</v>
@@ -3591,55 +3612,43 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>344</v>
+        <v>690</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K23" s="1" t="n">
-        <v>600000</v>
+        <v>132</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L23" s="1" t="n">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q23" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="S23" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T23" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="U23" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="V23" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="W23" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="X23" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="Y23" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z23" s="1" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="1" t="n">
         <v>1</v>
@@ -3675,16 +3684,16 @@
         <v>0</v>
       </c>
       <c r="BB23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF23" s="1" t="n">
         <v>0</v>
@@ -3710,22 +3719,25 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>691</v>
+        <v>300</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>5000</v>
+        <v>134</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L24" s="1" t="n">
         <v>1000000000</v>
@@ -3733,17 +3745,29 @@
       <c r="O24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" s="1" t="n">
-        <v>0.3</v>
+      <c r="S24" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="T24" s="1" t="n">
-        <v>0.55</v>
+        <v>0.7</v>
+      </c>
+      <c r="U24" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V24" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W24" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="X24" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y24" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Z24" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC24" s="1" t="n">
         <v>1</v>
@@ -3814,22 +3838,22 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>385</v>
+        <v>344</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K25" s="1" t="n">
         <v>600000</v>
@@ -3844,10 +3868,10 @@
         <v>0.15</v>
       </c>
       <c r="T25" s="1" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="U25" s="1" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="V25" s="1" t="n">
         <v>0.8</v>
@@ -3856,13 +3880,13 @@
         <v>0.8</v>
       </c>
       <c r="X25" s="1" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="Y25" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="Z25" s="1" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AC25" s="1" t="n">
         <v>1</v>
@@ -3933,25 +3957,22 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>427</v>
+        <v>691</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K26" s="1" t="n">
-        <v>600000</v>
+        <v>138</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L26" s="1" t="n">
         <v>1000000000</v>
@@ -3959,29 +3980,17 @@
       <c r="O26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S26" s="1" t="n">
-        <v>0.15</v>
+      <c r="Q26" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="T26" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="U26" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="V26" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="W26" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="X26" s="1" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="Y26" s="1" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC26" s="1" t="n">
         <v>1</v>
@@ -4052,22 +4061,25 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>694</v>
+        <v>385</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <v>5000</v>
+        <v>140</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>1000000000</v>
@@ -4075,17 +4087,29 @@
       <c r="O27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" s="1" t="n">
-        <v>0.3</v>
+      <c r="S27" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T27" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U27" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="V27" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W27" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X27" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y27" s="1" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="Z27" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC27" s="1" t="n">
         <v>1</v>
@@ -4156,28 +4180,25 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>469</v>
+        <v>427</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <v>2000000</v>
+        <v>110</v>
       </c>
       <c r="K28" s="1" t="n">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="L28" s="1" t="n">
         <v>1000000000</v>
@@ -4186,19 +4207,19 @@
         <v>0</v>
       </c>
       <c r="S28" s="1" t="n">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="T28" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="U28" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="V28" s="1" t="n">
         <v>0.8</v>
       </c>
       <c r="W28" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="X28" s="1" t="n">
         <v>0.7</v>
@@ -4278,43 +4299,34 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>681</v>
+        <v>694</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>250000000000</v>
-      </c>
-      <c r="M29" s="1" t="n">
-        <v>25000</v>
-      </c>
-      <c r="N29" s="1" t="n">
-        <v>2500</v>
+        <v>1000000000</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T29" s="1" t="n">
-        <v>0.55</v>
+        <v>0.3</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>0.55</v>
+        <v>0.7</v>
       </c>
       <c r="Y29" s="1" t="n">
         <v>0</v>
@@ -4374,7 +4386,7 @@
         <v>0</v>
       </c>
       <c r="BM29" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BN29" s="1" t="n">
         <v>0</v>
@@ -4391,46 +4403,58 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>684</v>
+        <v>469</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="H30" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="I30" s="1" t="n">
-        <v>3000</v>
+        <v>2000000</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>250000000000</v>
-      </c>
-      <c r="M30" s="1" t="n">
-        <v>25000</v>
-      </c>
-      <c r="N30" s="1" t="n">
-        <v>2500</v>
+        <v>1000000000</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="Q30" s="1" t="n">
-        <v>0.15</v>
+        <v>0</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="T30" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U30" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V30" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W30" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="X30" s="1" t="n">
-        <v>0.55</v>
+        <v>0.7</v>
       </c>
       <c r="Y30" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z30" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC30" s="1" t="n">
         <v>1</v>
@@ -4484,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="BM30" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BN30" s="1" t="n">
         <v>0</v>
@@ -4501,19 +4525,22 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>3000</v>
       </c>
       <c r="L31" s="1" t="n">
         <v>250000000000</v>
@@ -4527,14 +4554,20 @@
       <c r="O31" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="W31" s="1" t="n">
+      <c r="Q31" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T31" s="1" t="n">
         <v>0.55</v>
       </c>
+      <c r="V31" s="1" t="n">
+        <v>0.55</v>
+      </c>
       <c r="Y31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z31" s="1" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="1" t="n">
         <v>1</v>
@@ -4566,11 +4599,8 @@
       <c r="AY31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AZ31" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BA31" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB31" s="1" t="n">
         <v>0</v>
@@ -4608,22 +4638,22 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="L32" s="1" t="n">
         <v>250000000000</v>
@@ -4637,14 +4667,20 @@
       <c r="O32" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="X32" s="1" t="n">
+      <c r="Q32" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T32" s="1" t="n">
         <v>0.55</v>
       </c>
+      <c r="V32" s="1" t="n">
+        <v>0.55</v>
+      </c>
       <c r="Y32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z32" s="1" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="AC32" s="1" t="n">
         <v>1</v>
@@ -4715,25 +4751,22 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>226</v>
+        <v>684</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K33" s="1" t="n">
-        <v>500000</v>
+        <v>152</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>3000</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>250000000000</v>
@@ -4747,29 +4780,17 @@
       <c r="O33" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S33" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T33" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U33" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="V33" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="W33" s="1" t="n">
-        <v>0.4</v>
+      <c r="Q33" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="X33" s="1" t="n">
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="Y33" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="1" t="n">
         <v>1</v>
@@ -4840,22 +4861,19 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>267</v>
+        <v>686</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="K34" s="1" t="n">
-        <v>750000</v>
+        <v>154</v>
       </c>
       <c r="L34" s="1" t="n">
         <v>250000000000</v>
@@ -4869,17 +4887,14 @@
       <c r="O34" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S34" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="U34" s="1" t="n">
-        <v>0.7</v>
+      <c r="W34" s="1" t="n">
+        <v>0.55</v>
       </c>
       <c r="Y34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z34" s="1" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="AC34" s="1" t="n">
         <v>1</v>
@@ -4911,8 +4926,11 @@
       <c r="AY34" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ34" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA34" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB34" s="1" t="n">
         <v>0</v>
@@ -4950,28 +4968,22 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>678</v>
+        <v>689</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="L35" s="1" t="n">
         <v>250000000000</v>
@@ -4985,20 +4997,14 @@
       <c r="O35" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="Q35" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="R35" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="S35" s="1" t="n">
-        <v>0.7</v>
+      <c r="X35" s="1" t="n">
+        <v>0.55</v>
       </c>
       <c r="Y35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z35" s="1" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="AC35" s="1" t="n">
         <v>1</v>
@@ -5034,16 +5040,16 @@
         <v>0</v>
       </c>
       <c r="BB35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE35" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF35" s="1" t="n">
         <v>0</v>
@@ -5069,22 +5075,22 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>311</v>
+        <v>226</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K36" s="1" t="n">
         <v>500000</v>
@@ -5194,25 +5200,22 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>353</v>
+        <v>267</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>500000</v>
+        <v>750000</v>
       </c>
       <c r="L37" s="1" t="n">
         <v>250000000000</v>
@@ -5229,26 +5232,14 @@
       <c r="S37" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="T37" s="1" t="n">
-        <v>0.4</v>
-      </c>
       <c r="U37" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="V37" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="W37" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="X37" s="1" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="Y37" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z37" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="1" t="n">
         <v>1</v>
@@ -5319,22 +5310,28 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>3000</v>
+        <v>1000</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L38" s="1" t="n">
         <v>250000000000</v>
@@ -5349,10 +5346,13 @@
         <v>1000</v>
       </c>
       <c r="Q38" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T38" s="1" t="n">
-        <v>0.55</v>
+        <v>0.7</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="S38" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y38" s="1" t="n">
         <v>0</v>
@@ -5394,16 +5394,16 @@
         <v>0</v>
       </c>
       <c r="BB38" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC38" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD38" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE38" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF38" s="1" t="n">
         <v>0</v>
@@ -5429,22 +5429,22 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>397</v>
+        <v>311</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="K39" s="1" t="n">
         <v>500000</v>
@@ -5554,22 +5554,22 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>437</v>
+        <v>353</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="K40" s="1" t="n">
         <v>500000</v>
@@ -5679,19 +5679,19 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I41" s="1" t="n">
         <v>3000</v>
@@ -5711,7 +5711,7 @@
       <c r="Q41" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="V41" s="1" t="n">
+      <c r="T41" s="1" t="n">
         <v>0.55</v>
       </c>
       <c r="Y41" s="1" t="n">
@@ -5789,25 +5789,25 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>485</v>
+        <v>397</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K42" s="1" t="n">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="L42" s="1" t="n">
         <v>250000000000</v>
@@ -5825,25 +5825,25 @@
         <v>0.1</v>
       </c>
       <c r="T42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="U42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="V42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="W42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="X42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="Y42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="Z42" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="AC42" s="1" t="n">
         <v>1</v>
@@ -5912,45 +5912,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>679</v>
+        <v>437</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I43" s="1" t="n">
-        <v>5000</v>
+      <c r="H43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>500000</v>
       </c>
       <c r="L43" s="1" t="n">
-        <v>1000000000</v>
+        <v>250000000000</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>2500</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="1" t="n">
-        <v>0.35</v>
+        <v>1000</v>
+      </c>
+      <c r="S43" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="T43" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V43" s="2" t="n">
-        <v>0.75</v>
+        <v>0.4</v>
+      </c>
+      <c r="U43" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="V43" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W43" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X43" s="1" t="n">
+        <v>0.4</v>
       </c>
       <c r="Y43" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Z43" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AC43" s="1" t="n">
         <v>1</v>
@@ -6004,7 +6022,7 @@
         <v>0</v>
       </c>
       <c r="BM43" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN43" s="1" t="n">
         <v>0</v>
@@ -6019,36 +6037,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>682</v>
+        <v>696</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>174</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="L44" s="1" t="n">
-        <v>1000000000</v>
+        <v>250000000000</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N44" s="1" t="n">
+        <v>2500</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Q44" s="1" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="X44" s="2" t="n">
-        <v>0.75</v>
+        <v>0.15</v>
+      </c>
+      <c r="V44" s="1" t="n">
+        <v>0.55</v>
       </c>
       <c r="Y44" s="1" t="n">
         <v>0</v>
@@ -6108,7 +6132,7 @@
         <v>0</v>
       </c>
       <c r="BM44" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN44" s="1" t="n">
         <v>0</v>
@@ -6125,20 +6149,26 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>686</v>
+        <v>485</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>175</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>176</v>
       </c>
+      <c r="H45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>1000000</v>
+      </c>
       <c r="L45" s="1" t="n">
         <v>250000000000</v>
       </c>
@@ -6151,14 +6181,29 @@
       <c r="O45" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="S45" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T45" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="U45" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V45" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="W45" s="1" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
+      </c>
+      <c r="X45" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y45" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Z45" s="1" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="AC45" s="1" t="n">
         <v>1</v>
@@ -6190,11 +6235,8 @@
       <c r="AY45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AZ45" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BA45" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB45" s="1" t="n">
         <v>0</v>
@@ -6232,22 +6274,22 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>177</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>1000000</v>
+        <v>5000</v>
       </c>
       <c r="L46" s="1" t="n">
         <v>1000000000</v>
@@ -6256,16 +6298,19 @@
         <v>0</v>
       </c>
       <c r="Q46" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="X46" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T46" s="1" t="n">
         <v>0.75</v>
       </c>
+      <c r="V46" s="2" t="n">
+        <v>0.75</v>
+      </c>
       <c r="Y46" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z46" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC46" s="1" t="n">
         <v>1</v>
@@ -6336,25 +6381,22 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>213</v>
+        <v>679</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K47" s="1" t="n">
-        <v>600000</v>
+        <v>181</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L47" s="1" t="n">
         <v>1000000000</v>
@@ -6362,29 +6404,20 @@
       <c r="O47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S47" s="1" t="n">
-        <v>0.2</v>
+      <c r="Q47" s="1" t="n">
+        <v>0.35</v>
       </c>
       <c r="T47" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="U47" s="1" t="n">
+      <c r="V47" s="2" t="n">
         <v>0.75</v>
       </c>
-      <c r="V47" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="W47" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="X47" s="1" t="n">
-        <v>0.75</v>
-      </c>
       <c r="Y47" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC47" s="1" t="n">
         <v>1</v>
@@ -6455,22 +6488,22 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>258</v>
+        <v>682</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K48" s="1" t="n">
-        <v>1000000</v>
+        <v>183</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L48" s="1" t="n">
         <v>1000000000</v>
@@ -6478,11 +6511,11 @@
       <c r="O48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S48" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="U48" s="1" t="n">
-        <v>0.8</v>
+      <c r="Q48" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="X48" s="2" t="n">
+        <v>0.75</v>
       </c>
       <c r="Y48" s="1" t="n">
         <v>0</v>
@@ -6557,45 +6590,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="I49" s="1" t="n">
-        <v>5000</v>
+        <v>185</v>
       </c>
       <c r="L49" s="1" t="n">
-        <v>1000000</v>
+        <v>250000000000</v>
+      </c>
+      <c r="M49" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N49" s="1" t="n">
+        <v>2500</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="R49" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="S49" s="1" t="n">
-        <v>0.85</v>
+        <v>1000</v>
+      </c>
+      <c r="W49" s="1" t="n">
+        <v>0.6</v>
       </c>
       <c r="Y49" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z49" s="1" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AC49" s="1" t="n">
         <v>1</v>
@@ -6627,20 +6657,23 @@
       <c r="AY49" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ49" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA49" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB49" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC49" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD49" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE49" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF49" s="1" t="n">
         <v>0</v>
@@ -6649,7 +6682,7 @@
         <v>0</v>
       </c>
       <c r="BM49" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN49" s="1" t="n">
         <v>0</v>
@@ -6666,25 +6699,22 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>300</v>
+        <v>687</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K50" s="1" t="n">
-        <v>600000</v>
+        <v>187</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L50" s="1" t="n">
         <v>1000000000</v>
@@ -6692,29 +6722,17 @@
       <c r="O50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S50" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="T50" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="U50" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V50" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="W50" s="1" t="n">
-        <v>0.75</v>
+      <c r="Q50" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="X50" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="Y50" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="AC50" s="1" t="n">
         <v>1</v>
@@ -6785,22 +6803,22 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>344</v>
+        <v>213</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="K51" s="1" t="n">
         <v>600000</v>
@@ -6815,25 +6833,25 @@
         <v>0.2</v>
       </c>
       <c r="T51" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="U51" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="V51" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="W51" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="X51" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="Y51" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="Z51" s="1" t="n">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="AC51" s="1" t="n">
         <v>1</v>
@@ -6904,22 +6922,22 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>691</v>
+        <v>258</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I52" s="1" t="n">
-        <v>5000</v>
+        <v>191</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L52" s="1" t="n">
         <v>1000000000</v>
@@ -6927,11 +6945,11 @@
       <c r="O52" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q52" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="T52" s="1" t="n">
-        <v>0.6</v>
+      <c r="S52" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U52" s="1" t="n">
+        <v>0.8</v>
       </c>
       <c r="Y52" s="1" t="n">
         <v>0</v>
@@ -7008,55 +7026,43 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>385</v>
+        <v>690</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K53" s="1" t="n">
-        <v>600000</v>
+        <v>193</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L53" s="1" t="n">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="O53" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q53" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="R53" s="1" t="n">
+        <v>0.75</v>
+      </c>
       <c r="S53" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="T53" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="U53" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="V53" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="W53" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="X53" s="1" t="n">
-        <v>0.75</v>
-      </c>
       <c r="Y53" s="1" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="Z53" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AC53" s="1" t="n">
         <v>1</v>
@@ -7092,16 +7098,16 @@
         <v>0</v>
       </c>
       <c r="BB53" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC53" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD53" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE53" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF53" s="1" t="n">
         <v>0</v>
@@ -7127,22 +7133,22 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>427</v>
+        <v>300</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="K54" s="1" t="n">
         <v>600000</v>
@@ -7157,13 +7163,13 @@
         <v>0.2</v>
       </c>
       <c r="T54" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="U54" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="V54" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="W54" s="1" t="n">
         <v>0.75</v>
@@ -7172,10 +7178,10 @@
         <v>0.75</v>
       </c>
       <c r="Y54" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="Z54" s="1" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="AC54" s="1" t="n">
         <v>1</v>
@@ -7246,22 +7252,25 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>694</v>
+        <v>344</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I55" s="1" t="n">
-        <v>5000</v>
+        <v>197</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L55" s="1" t="n">
         <v>1000000000</v>
@@ -7269,17 +7278,29 @@
       <c r="O55" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q55" s="1" t="n">
-        <v>0.3</v>
+      <c r="S55" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T55" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U55" s="1" t="n">
+        <v>0.85</v>
       </c>
       <c r="V55" s="1" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
+      </c>
+      <c r="W55" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X55" s="1" t="n">
+        <v>0.8</v>
       </c>
       <c r="Y55" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z55" s="1" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AC55" s="1" t="n">
         <v>1</v>
@@ -7350,26 +7371,22 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>469</v>
+        <v>691</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I56" s="0"/>
-      <c r="K56" s="1" t="n">
-        <v>2000000</v>
+        <v>199</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L56" s="1" t="n">
         <v>1000000000</v>
@@ -7377,94 +7394,543 @@
       <c r="O56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S56" s="1" t="n">
+      <c r="Q56" s="1" t="n">
         <v>0.3</v>
       </c>
       <c r="T56" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ56" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L57" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T57" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U57" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V57" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="U56" s="1" t="n">
+      <c r="W57" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X57" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y57" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="V56" s="1" t="n">
+      <c r="Z57" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AC57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ57" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L58" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T58" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U58" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V58" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="W56" s="1" t="n">
+      <c r="W58" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X58" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y58" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Z58" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ58" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>694</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L59" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V59" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ59" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L60" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T60" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U60" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="X56" s="1" t="n">
+      <c r="V60" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W60" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X60" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="Y56" s="1" t="n">
+      <c r="Y60" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="Z56" s="1" t="n">
+      <c r="Z60" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="AC56" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ56" s="1" t="n">
+      <c r="AC60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ60" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished implementing the new tables for the public facing info pages.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="237">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t xml:space="preserve">Pillage and plunder. Steal and stab. Take whats yours, no matter the cost!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call of The Sea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The call of the sea will heal the wounds of the desolate</t>
   </si>
   <si>
     <t xml:space="preserve">Pirate Leather Sleeves</t>
@@ -1009,10 +1015,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT72"/>
+  <dimension ref="A1:BT73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J62" activeCellId="0" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4134,13 +4140,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>213</v>
+        <v>687</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>128</v>
@@ -4148,11 +4154,9 @@
       <c r="G27" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K27" s="1" t="n">
-        <v>600000</v>
+      <c r="I27" s="0"/>
+      <c r="J27" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L27" s="1" t="n">
         <v>1000000000</v>
@@ -4160,26 +4164,14 @@
       <c r="O27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S27" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T27" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="U27" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="V27" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="W27" s="1" t="n">
-        <v>0.7</v>
+      <c r="Q27" s="1" t="n">
+        <v>0.25</v>
       </c>
       <c r="X27" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y27" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z27" s="1" t="n">
         <v>0.7</v>
@@ -4214,8 +4206,11 @@
       <c r="AY27" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ27" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA27" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB27" s="1" t="n">
         <v>0</v>
@@ -4253,13 +4248,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>128</v>
@@ -4267,8 +4262,11 @@
       <c r="G28" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="H28" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="K28" s="1" t="n">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="L28" s="1" t="n">
         <v>1000000000</v>
@@ -4279,14 +4277,26 @@
       <c r="S28" s="1" t="n">
         <v>0.15</v>
       </c>
+      <c r="T28" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="U28" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
+      </c>
+      <c r="V28" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W28" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="X28" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y28" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Z28" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC28" s="1" t="n">
         <v>1</v>
@@ -4357,13 +4367,13 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>690</v>
+        <v>258</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>128</v>
@@ -4371,24 +4381,21 @@
       <c r="G29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I29" s="1" t="n">
-        <v>5000</v>
+      <c r="K29" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="O29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" s="1" t="n">
+      <c r="S29" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="U29" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="R29" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="S29" s="1" t="n">
-        <v>0.75</v>
-      </c>
       <c r="Y29" s="1" t="n">
         <v>0</v>
       </c>
@@ -4429,16 +4436,16 @@
         <v>0</v>
       </c>
       <c r="BB29" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC29" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD29" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE29" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF29" s="1" t="n">
         <v>0</v>
@@ -4464,13 +4471,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>300</v>
+        <v>690</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>128</v>
@@ -4478,41 +4485,29 @@
       <c r="G30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K30" s="1" t="n">
-        <v>600000</v>
+      <c r="I30" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q30" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="R30" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="S30" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="T30" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="U30" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="V30" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="W30" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="X30" s="1" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="Y30" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC30" s="1" t="n">
         <v>1</v>
@@ -4548,16 +4543,16 @@
         <v>0</v>
       </c>
       <c r="BB30" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC30" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD30" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE30" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF30" s="1" t="n">
         <v>0</v>
@@ -4583,13 +4578,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>344</v>
+        <v>300</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>128</v>
@@ -4598,7 +4593,7 @@
         <v>151</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K31" s="1" t="n">
         <v>600000</v>
@@ -4613,25 +4608,25 @@
         <v>0.15</v>
       </c>
       <c r="T31" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="U31" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="X31" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="Y31" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="Z31" s="1" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AC31" s="1" t="n">
         <v>1</v>
@@ -4700,15 +4695,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>691</v>
+        <v>344</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>128</v>
@@ -4716,8 +4711,11 @@
       <c r="G32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I32" s="1" t="n">
-        <v>5000</v>
+      <c r="H32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L32" s="1" t="n">
         <v>1000000000</v>
@@ -4725,17 +4723,29 @@
       <c r="O32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" s="1" t="n">
-        <v>0.3</v>
+      <c r="S32" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="T32" s="1" t="n">
-        <v>0.55</v>
+        <v>0.8</v>
+      </c>
+      <c r="U32" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V32" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W32" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X32" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="Y32" s="1" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="Z32" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AC32" s="1" t="n">
         <v>1</v>
@@ -4804,15 +4814,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>385</v>
+        <v>691</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>128</v>
@@ -4820,11 +4830,8 @@
       <c r="G33" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K33" s="1" t="n">
-        <v>600000</v>
+      <c r="I33" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L33" s="1" t="n">
         <v>1000000000</v>
@@ -4832,29 +4839,17 @@
       <c r="O33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S33" s="1" t="n">
-        <v>0.15</v>
+      <c r="Q33" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="T33" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="U33" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V33" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="W33" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="X33" s="1" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="Y33" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="1" t="n">
         <v>1</v>
@@ -4925,13 +4920,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>427</v>
+        <v>385</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>156</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>128</v>
@@ -4940,7 +4935,7 @@
         <v>157</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K34" s="1" t="n">
         <v>600000</v>
@@ -4958,19 +4953,19 @@
         <v>0.75</v>
       </c>
       <c r="U34" s="1" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="V34" s="1" t="n">
         <v>0.8</v>
       </c>
       <c r="W34" s="1" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="X34" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y34" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="Z34" s="1" t="n">
         <v>0.7</v>
@@ -5044,13 +5039,13 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>694</v>
+        <v>427</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>128</v>
@@ -5058,8 +5053,11 @@
       <c r="G35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I35" s="1" t="n">
-        <v>5000</v>
+      <c r="H35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L35" s="1" t="n">
         <v>1000000000</v>
@@ -5067,17 +5065,29 @@
       <c r="O35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" s="1" t="n">
-        <v>0.3</v>
+      <c r="S35" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="T35" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U35" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="V35" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W35" s="1" t="n">
         <v>0.7</v>
       </c>
+      <c r="X35" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="Y35" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z35" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC35" s="1" t="n">
         <v>1</v>
@@ -5146,30 +5156,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>469</v>
+        <v>694</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="K36" s="1" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L36" s="1" t="n">
         <v>1000000000</v>
@@ -5177,29 +5181,17 @@
       <c r="O36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S36" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="T36" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="U36" s="1" t="n">
-        <v>0.75</v>
+      <c r="Q36" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="V36" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="W36" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="X36" s="1" t="n">
         <v>0.7</v>
       </c>
       <c r="Y36" s="1" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="1" t="n">
         <v>1</v>
@@ -5270,49 +5262,58 @@
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>681</v>
+        <v>469</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>163</v>
+      <c r="H37" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>3000</v>
+        <v>2000000</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L37" s="1" t="n">
-        <v>250000000000</v>
-      </c>
-      <c r="M37" s="1" t="n">
-        <v>25000</v>
-      </c>
-      <c r="N37" s="1" t="n">
-        <v>2500</v>
+        <v>1000000000</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="Q37" s="1" t="n">
-        <v>0.15</v>
+        <v>0</v>
+      </c>
+      <c r="S37" s="1" t="n">
+        <v>0.25</v>
       </c>
       <c r="T37" s="1" t="n">
-        <v>0.55</v>
+        <v>0.8</v>
+      </c>
+      <c r="U37" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="V37" s="1" t="n">
-        <v>0.55</v>
+        <v>0.8</v>
+      </c>
+      <c r="W37" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X37" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y37" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z37" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC37" s="1" t="n">
         <v>1</v>
@@ -5366,7 +5367,7 @@
         <v>0</v>
       </c>
       <c r="BM37" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BN37" s="1" t="n">
         <v>0</v>
@@ -5381,18 +5382,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>681</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>165</v>
@@ -5494,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>681</v>
       </c>
@@ -5502,10 +5503,10 @@
         <v>166</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>167</v>
@@ -5615,10 +5616,10 @@
         <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>169</v>
@@ -5728,10 +5729,10 @@
         <v>170</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>171</v>
@@ -5835,16 +5836,16 @@
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>172</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>173</v>
@@ -5867,7 +5868,10 @@
       <c r="Q42" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="X42" s="1" t="n">
+      <c r="T42" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="V42" s="1" t="n">
         <v>0.55</v>
       </c>
       <c r="Y42" s="1" t="n">
@@ -5945,20 +5949,23 @@
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>174</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>175</v>
       </c>
+      <c r="I43" s="1" t="n">
+        <v>3000</v>
+      </c>
       <c r="L43" s="1" t="n">
         <v>250000000000</v>
       </c>
@@ -5971,14 +5978,17 @@
       <c r="O43" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="W43" s="1" t="n">
+      <c r="Q43" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="X43" s="1" t="n">
         <v>0.55</v>
       </c>
       <c r="Y43" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z43" s="1" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="AC43" s="1" t="n">
         <v>1</v>
@@ -6010,11 +6020,8 @@
       <c r="AY43" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AZ43" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BA43" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB43" s="1" t="n">
         <v>0</v>
@@ -6052,21 +6059,21 @@
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I44" s="1" t="n">
+      <c r="J44" s="1" t="n">
         <v>10000</v>
       </c>
       <c r="L44" s="1" t="n">
@@ -6081,7 +6088,7 @@
       <c r="O44" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="X44" s="1" t="n">
+      <c r="W44" s="1" t="n">
         <v>0.55</v>
       </c>
       <c r="Y44" s="1" t="n">
@@ -6120,8 +6127,11 @@
       <c r="AY44" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ44" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA44" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB44" s="1" t="n">
         <v>0</v>
@@ -6159,25 +6169,22 @@
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>226</v>
+        <v>689</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>178</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K45" s="1" t="n">
-        <v>500000</v>
+      <c r="I45" s="1" t="n">
+        <v>10000</v>
       </c>
       <c r="L45" s="1" t="n">
         <v>250000000000</v>
@@ -6191,29 +6198,14 @@
       <c r="O45" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S45" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T45" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U45" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="V45" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="W45" s="1" t="n">
-        <v>0.4</v>
-      </c>
       <c r="X45" s="1" t="n">
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="Y45" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z45" s="1" t="n">
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="AC45" s="1" t="n">
         <v>1</v>
@@ -6284,22 +6276,25 @@
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>267</v>
+        <v>226</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>180</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="H46" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="K46" s="1" t="n">
-        <v>750000</v>
+        <v>500000</v>
       </c>
       <c r="L46" s="1" t="n">
         <v>250000000000</v>
@@ -6316,14 +6311,26 @@
       <c r="S46" s="1" t="n">
         <v>0.1</v>
       </c>
+      <c r="T46" s="1" t="n">
+        <v>0.4</v>
+      </c>
       <c r="U46" s="1" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
+      </c>
+      <c r="V46" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W46" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X46" s="1" t="n">
+        <v>0.4</v>
       </c>
       <c r="Y46" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Z46" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AC46" s="1" t="n">
         <v>1</v>
@@ -6392,30 +6399,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>678</v>
+        <v>267</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>182</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I47" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J47" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="K47" s="1" t="n">
-        <v>0</v>
+        <v>750000</v>
       </c>
       <c r="L47" s="1" t="n">
         <v>250000000000</v>
@@ -6429,15 +6430,12 @@
       <c r="O47" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="Q47" s="1" t="n">
+      <c r="S47" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U47" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="R47" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="S47" s="1" t="n">
-        <v>0.7</v>
-      </c>
       <c r="Y47" s="1" t="n">
         <v>0</v>
       </c>
@@ -6478,16 +6476,16 @@
         <v>0</v>
       </c>
       <c r="BB47" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC47" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD47" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE47" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF47" s="1" t="n">
         <v>0</v>
@@ -6511,27 +6509,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>311</v>
+        <v>678</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>184</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>107</v>
+      <c r="I48" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="L48" s="1" t="n">
         <v>250000000000</v>
@@ -6545,29 +6546,20 @@
       <c r="O48" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="Q48" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="R48" s="1" t="n">
+        <v>0.7</v>
+      </c>
       <c r="S48" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T48" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U48" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="V48" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="W48" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="X48" s="1" t="n">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="Y48" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z48" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="1" t="n">
         <v>1</v>
@@ -6603,16 +6595,16 @@
         <v>0</v>
       </c>
       <c r="BB48" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC48" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD48" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE48" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF48" s="1" t="n">
         <v>0</v>
@@ -6636,24 +6628,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>186</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>187</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K49" s="1" t="n">
         <v>500000</v>
@@ -6761,24 +6753,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>693</v>
+        <v>353</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>188</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I50" s="1" t="n">
-        <v>3000</v>
+      <c r="H50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K50" s="1" t="n">
+        <v>500000</v>
       </c>
       <c r="L50" s="1" t="n">
         <v>250000000000</v>
@@ -6792,17 +6787,29 @@
       <c r="O50" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="Q50" s="1" t="n">
-        <v>0.15</v>
+      <c r="S50" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="T50" s="1" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
+      </c>
+      <c r="U50" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="V50" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="W50" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X50" s="1" t="n">
+        <v>0.4</v>
       </c>
       <c r="Y50" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Z50" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AC50" s="1" t="n">
         <v>1</v>
@@ -6871,27 +6878,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>397</v>
+        <v>693</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>190</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K51" s="1" t="n">
-        <v>500000</v>
+      <c r="I51" s="1" t="n">
+        <v>3000</v>
       </c>
       <c r="L51" s="1" t="n">
         <v>250000000000</v>
@@ -6905,29 +6909,17 @@
       <c r="O51" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S51" s="1" t="n">
-        <v>0.1</v>
+      <c r="Q51" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="T51" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="U51" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="V51" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="W51" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="X51" s="1" t="n">
-        <v>0.4</v>
+        <v>0.55</v>
       </c>
       <c r="Y51" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z51" s="1" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AC51" s="1" t="n">
         <v>1</v>
@@ -6998,22 +6990,22 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>192</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>193</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K52" s="1" t="n">
         <v>500000</v>
@@ -7123,22 +7115,25 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>696</v>
+        <v>437</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>194</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="I53" s="1" t="n">
-        <v>3000</v>
+      <c r="H53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>500000</v>
       </c>
       <c r="L53" s="1" t="n">
         <v>250000000000</v>
@@ -7152,17 +7147,29 @@
       <c r="O53" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="Q53" s="1" t="n">
-        <v>0.15</v>
+      <c r="S53" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T53" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U53" s="1" t="n">
+        <v>0.4</v>
       </c>
       <c r="V53" s="1" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
+      </c>
+      <c r="W53" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X53" s="1" t="n">
+        <v>0.4</v>
       </c>
       <c r="Y53" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Z53" s="1" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AC53" s="1" t="n">
         <v>1</v>
@@ -7233,25 +7240,22 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>485</v>
+        <v>696</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>196</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K54" s="1" t="n">
-        <v>1000000</v>
+      <c r="I54" s="1" t="n">
+        <v>3000</v>
       </c>
       <c r="L54" s="1" t="n">
         <v>250000000000</v>
@@ -7265,29 +7269,17 @@
       <c r="O54" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="S54" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T54" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="U54" s="1" t="n">
-        <v>0.7</v>
+      <c r="Q54" s="1" t="n">
+        <v>0.15</v>
       </c>
       <c r="V54" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="W54" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="X54" s="1" t="n">
-        <v>0.7</v>
+        <v>0.55</v>
       </c>
       <c r="Y54" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="Z54" s="1" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="AC54" s="1" t="n">
         <v>1</v>
@@ -7358,43 +7350,61 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>679</v>
+        <v>485</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>198</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I55" s="1" t="n">
-        <v>5000</v>
+      <c r="H55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L55" s="1" t="n">
-        <v>1000000000</v>
+        <v>250000000000</v>
+      </c>
+      <c r="M55" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N55" s="1" t="n">
+        <v>2500</v>
       </c>
       <c r="O55" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="1" t="n">
-        <v>0.35</v>
+        <v>1000</v>
+      </c>
+      <c r="S55" s="1" t="n">
+        <v>0.1</v>
       </c>
       <c r="T55" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V55" s="3" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
+      </c>
+      <c r="U55" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V55" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W55" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="X55" s="1" t="n">
+        <v>0.7</v>
       </c>
       <c r="Y55" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="Z55" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC55" s="1" t="n">
         <v>1</v>
@@ -7448,7 +7458,7 @@
         <v>0</v>
       </c>
       <c r="BM55" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN55" s="1" t="n">
         <v>0</v>
@@ -7468,13 +7478,13 @@
         <v>679</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>202</v>
@@ -7578,10 +7588,10 @@
         <v>203</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>204</v>
@@ -7685,10 +7695,10 @@
         <v>205</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>206</v>
@@ -7792,10 +7802,10 @@
         <v>207</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>208</v>
@@ -7893,16 +7903,16 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>209</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>210</v>
@@ -7919,7 +7929,10 @@
       <c r="Q60" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="X60" s="3" t="n">
+      <c r="T60" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V60" s="3" t="n">
         <v>0.75</v>
       </c>
       <c r="Y60" s="1" t="n">
@@ -7997,40 +8010,40 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>212</v>
       </c>
+      <c r="I61" s="1" t="n">
+        <v>5000</v>
+      </c>
       <c r="L61" s="1" t="n">
-        <v>250000000000</v>
-      </c>
-      <c r="M61" s="1" t="n">
-        <v>25000</v>
-      </c>
-      <c r="N61" s="1" t="n">
-        <v>2500</v>
+        <v>1000000000</v>
       </c>
       <c r="O61" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="W61" s="1" t="n">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="Q61" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="X61" s="3" t="n">
+        <v>0.75</v>
       </c>
       <c r="Y61" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z61" s="1" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AC61" s="1" t="n">
         <v>1</v>
@@ -8062,11 +8075,8 @@
       <c r="AY61" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AZ61" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="BA61" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB61" s="1" t="n">
         <v>0</v>
@@ -8087,7 +8097,7 @@
         <v>0</v>
       </c>
       <c r="BM61" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="BN61" s="1" t="n">
         <v>0</v>
@@ -8104,40 +8114,43 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>213</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="I62" s="1" t="n">
+      <c r="J62" s="1" t="n">
         <v>1000000</v>
       </c>
       <c r="L62" s="1" t="n">
-        <v>1000000000</v>
+        <v>250000000000</v>
+      </c>
+      <c r="M62" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N62" s="1" t="n">
+        <v>2500</v>
       </c>
       <c r="O62" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="X62" s="1" t="n">
-        <v>0.75</v>
+        <v>1000</v>
+      </c>
+      <c r="W62" s="1" t="n">
+        <v>0.6</v>
       </c>
       <c r="Y62" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Z62" s="1" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AC62" s="1" t="n">
         <v>1</v>
@@ -8169,8 +8182,11 @@
       <c r="AY62" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="AZ62" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="BA62" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB62" s="1" t="n">
         <v>0</v>
@@ -8191,7 +8207,7 @@
         <v>0</v>
       </c>
       <c r="BM62" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN62" s="1" t="n">
         <v>0</v>
@@ -8208,25 +8224,22 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>213</v>
+        <v>687</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>215</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K63" s="1" t="n">
-        <v>600000</v>
+      <c r="I63" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L63" s="1" t="n">
         <v>1000000000</v>
@@ -8234,26 +8247,14 @@
       <c r="O63" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S63" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="T63" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="U63" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V63" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="W63" s="1" t="n">
-        <v>0.75</v>
+      <c r="Q63" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="X63" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="Y63" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z63" s="1" t="n">
         <v>0.7</v>
@@ -8327,22 +8328,25 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>217</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>218</v>
       </c>
+      <c r="H64" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="K64" s="1" t="n">
-        <v>1000000</v>
+        <v>600000</v>
       </c>
       <c r="L64" s="1" t="n">
         <v>1000000000</v>
@@ -8353,14 +8357,26 @@
       <c r="S64" s="1" t="n">
         <v>0.2</v>
       </c>
+      <c r="T64" s="1" t="n">
+        <v>0.75</v>
+      </c>
       <c r="U64" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
+      </c>
+      <c r="V64" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="W64" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X64" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="Y64" s="1" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="Z64" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC64" s="1" t="n">
         <v>1</v>
@@ -8431,37 +8447,34 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>690</v>
+        <v>258</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>219</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I65" s="1" t="n">
-        <v>5000</v>
+      <c r="K65" s="1" t="n">
+        <v>1000000</v>
       </c>
       <c r="L65" s="1" t="n">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
       <c r="O65" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q65" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="R65" s="1" t="n">
-        <v>0.75</v>
-      </c>
       <c r="S65" s="1" t="n">
-        <v>0.85</v>
+        <v>0.2</v>
+      </c>
+      <c r="U65" s="1" t="n">
+        <v>0.8</v>
       </c>
       <c r="Y65" s="1" t="n">
         <v>0</v>
@@ -8503,16 +8516,16 @@
         <v>0</v>
       </c>
       <c r="BB65" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC65" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD65" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE65" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF65" s="1" t="n">
         <v>0</v>
@@ -8538,55 +8551,43 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>300</v>
+        <v>690</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="K66" s="1" t="n">
-        <v>600000</v>
+      <c r="I66" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L66" s="1" t="n">
-        <v>1000000000</v>
+        <v>1000000</v>
       </c>
       <c r="O66" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q66" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="R66" s="1" t="n">
+        <v>0.75</v>
+      </c>
       <c r="S66" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="T66" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="U66" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="V66" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="W66" s="1" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="X66" s="1" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="Y66" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="Z66" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AC66" s="1" t="n">
         <v>1</v>
@@ -8622,16 +8623,16 @@
         <v>0</v>
       </c>
       <c r="BB66" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC66" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD66" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE66" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF66" s="1" t="n">
         <v>0</v>
@@ -8657,22 +8658,22 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>344</v>
+        <v>300</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>223</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>224</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K67" s="1" t="n">
         <v>600000</v>
@@ -8687,25 +8688,25 @@
         <v>0.2</v>
       </c>
       <c r="T67" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="U67" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="V67" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="W67" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="X67" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="Y67" s="1" t="n">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="Z67" s="1" t="n">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="AC67" s="1" t="n">
         <v>1</v>
@@ -8776,22 +8777,25 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>691</v>
+        <v>344</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>225</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I68" s="1" t="n">
-        <v>5000</v>
+      <c r="H68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K68" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L68" s="1" t="n">
         <v>1000000000</v>
@@ -8799,17 +8803,29 @@
       <c r="O68" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q68" s="1" t="n">
-        <v>0.3</v>
+      <c r="S68" s="1" t="n">
+        <v>0.2</v>
       </c>
       <c r="T68" s="1" t="n">
-        <v>0.6</v>
+        <v>0.85</v>
+      </c>
+      <c r="U68" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="V68" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W68" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X68" s="1" t="n">
+        <v>0.8</v>
       </c>
       <c r="Y68" s="1" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Z68" s="1" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AC68" s="1" t="n">
         <v>1</v>
@@ -8880,25 +8896,22 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>385</v>
+        <v>691</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H69" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K69" s="1" t="n">
-        <v>600000</v>
+      <c r="I69" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L69" s="1" t="n">
         <v>1000000000</v>
@@ -8906,29 +8919,17 @@
       <c r="O69" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S69" s="1" t="n">
-        <v>0.2</v>
+      <c r="Q69" s="1" t="n">
+        <v>0.3</v>
       </c>
       <c r="T69" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="U69" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="V69" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="W69" s="1" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="X69" s="1" t="n">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="Y69" s="1" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="Z69" s="1" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AC69" s="1" t="n">
         <v>1</v>
@@ -8999,22 +9000,22 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>427</v>
+        <v>385</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>229</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>230</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K70" s="1" t="n">
         <v>600000</v>
@@ -9032,22 +9033,22 @@
         <v>0.8</v>
       </c>
       <c r="U70" s="1" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="V70" s="1" t="n">
         <v>0.85</v>
       </c>
       <c r="W70" s="1" t="n">
-        <v>0.75</v>
+        <v>0.85</v>
       </c>
       <c r="X70" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="Y70" s="1" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="Z70" s="1" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="AC70" s="1" t="n">
         <v>1</v>
@@ -9118,22 +9119,25 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>694</v>
+        <v>427</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="I71" s="1" t="n">
-        <v>5000</v>
+      <c r="H71" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K71" s="1" t="n">
+        <v>600000</v>
       </c>
       <c r="L71" s="1" t="n">
         <v>1000000000</v>
@@ -9141,17 +9145,29 @@
       <c r="O71" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q71" s="1" t="n">
-        <v>0.3</v>
+      <c r="S71" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T71" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U71" s="1" t="n">
+        <v>0.75</v>
       </c>
       <c r="V71" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W71" s="1" t="n">
         <v>0.75</v>
       </c>
+      <c r="X71" s="1" t="n">
+        <v>0.75</v>
+      </c>
       <c r="Y71" s="1" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="Z71" s="1" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AC71" s="1" t="n">
         <v>1</v>
@@ -9222,25 +9238,22 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>469</v>
+        <v>694</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>233</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="K72" s="1" t="n">
-        <v>2000000</v>
+      <c r="I72" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="L72" s="1" t="n">
         <v>1000000000</v>
@@ -9248,94 +9261,201 @@
       <c r="O72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S72" s="1" t="n">
+      <c r="Q72" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="T72" s="1" t="n">
+      <c r="V72" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ72" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K73" s="1" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L73" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T73" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="U72" s="1" t="n">
+      <c r="U73" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="V72" s="1" t="n">
+      <c r="V73" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="W72" s="1" t="n">
+      <c r="W73" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="X72" s="1" t="n">
+      <c r="X73" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="Y72" s="1" t="n">
+      <c r="Y73" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="Z72" s="1" t="n">
+      <c r="Z73" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="AC72" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BA72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP72" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ72" s="1" t="n">
+      <c r="AC73" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ73" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More updates - new monster types added.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="274">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -731,6 +731,117 @@
   </si>
   <si>
     <t xml:space="preserve">Plate mail made of pure Ice. That was corrupted by tormented memories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earths Sword of Twisted Hate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sword born of the earth and twisted into a hate unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistol of the Vines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A gun of the vines that shoots the bullets of wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jungle Leaf Fans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fans for the dancers, made of giant but sturdy jungle leaves. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earths Blessed Mace of The Mother</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mace blessed of the mother of the earth her self.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted Corrupted Family of the Awl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A scratch awl that contains the families memories, twisted and broken as they are.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necromancers Stave of the Alchemist God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A necromancers stave that was given by a god of Alchemy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earths Healing Embrace III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let the earth embrace and heal your wounds child.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winds of rage and hate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let the winds of the east rage against the setting sun of the west.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleeves of the woods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleeves made of wood born of the earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shield of bark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A sturdy shield carved of thick bark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairy Wing Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A ring of the fairy creatures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rivers flowing leggings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leggings made of the flowing river stones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted helmet of illusions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A helmet that will twist and warp your mind to it’s own desires.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hammer of the ancients trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A hammer created from ancient trees harvest thousands of years ago. The wood never rots.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mossy Gloves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloves made of the softest moss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow Vines Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vines that wrap them selves in shadows to create boots for you to ware.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elven Bow of Seeing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bow created by the elves, one that grants you the gift of sight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natures Chain Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natures own chain mail crafted of the finest metals.</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1126,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT73"/>
+  <dimension ref="A1:BT91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J62" activeCellId="0" sqref="J62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G91" activeCellId="0" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4154,7 +4265,6 @@
       <c r="G27" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I27" s="0"/>
       <c r="J27" s="1" t="n">
         <v>1000000</v>
       </c>
@@ -9456,6 +9566,1992 @@
         <v>0</v>
       </c>
       <c r="BQ73" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L74" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T74" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V74" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ74" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L75" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T75" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V75" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC75" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ75" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L76" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T76" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V76" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ76" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L77" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T77" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V77" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ77" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="T78" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V78" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ78" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>682</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L79" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="1" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="X79" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ79" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="n">
+        <v>686</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L80" s="1" t="n">
+        <v>250000000000</v>
+      </c>
+      <c r="M80" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N80" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="O80" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W80" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AC80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM80" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ80" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L81" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="X81" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC81" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ81" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K82" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L82" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="W82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y82" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Z82" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ82" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K83" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="L83" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="U83" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ83" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>690</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L84" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="O84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="R84" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="S84" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Y84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ84" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K85" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L85" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="W85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Z85" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AC85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ85" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K86" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L86" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T86" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U86" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="V86" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W86" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X86" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y86" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Z86" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="AC86" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP86" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ86" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L87" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T87" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP87" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ87" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K88" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L88" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T88" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U88" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V88" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W88" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X88" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y88" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Z88" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AC88" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP88" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ88" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K89" s="1" t="n">
+        <v>600000</v>
+      </c>
+      <c r="L89" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="T89" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U89" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V89" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W89" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="X89" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y89" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Z89" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC89" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP89" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ89" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="n">
+        <v>694</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L90" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V90" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP90" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ90" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K91" s="1" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="L91" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T91" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U91" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V91" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W91" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X91" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="Y91" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Z91" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AC91" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP91" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ91" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing tests, trying to get things running again
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="311">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -842,6 +842,117 @@
   </si>
   <si>
     <t xml:space="preserve">Natures own chain mail crafted of the finest metals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Axe of Delusional Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An axe that resonated with delusional memories and twisted screams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow shotgun of the memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shot gun laced with the memories of a shadow. A shadow of pain.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Fans of Twisted Delusions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A simple silver fan that when used will show the enemy a series of twisted delusions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clerics Mace of Religious Zeolt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mace full of the religious zealots thoughts and twisted emotions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Book Binders Awl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A book binder ravaged with delusions and twisted emotions created his own tools out of madness.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Mages Red wood Stave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A simple red wood stave crafted by corrupted magics that have been manipulated by those of The Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal the mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal your mind of the corruption child.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravage the mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ravage the enemies body and mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver chain sleeves of delusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleeves made of chain that sparkles with twisted hate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shield of twisted delusions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shield of ones own twisted delusions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ring of fated child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A ring that once belonged to a child fated for Ascension.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Hawk Soldier Leggings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leggings worn by the Red Hawk soldiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Knight Helmet of The Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A holy helm of The Church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clerics Hammer of Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crafted in corrupt and delusional and twisted magics, this hammer is used by Clerics of a corrupted land.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silver Plate Gloves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beautifully polished silver plate gloves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional boots of yesterday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boots that will transport you back to the time of yesterday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted bow of time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bow that will twisted time and space around it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Silver Plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set of plate male that is crafted with the delusions of a broken man.</t>
   </si>
 </sst>
 </file>
@@ -851,7 +962,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -872,6 +983,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -917,7 +1034,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -931,6 +1048,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1126,10 +1251,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT91"/>
+  <dimension ref="A1:BT109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G91" activeCellId="0" sqref="G91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K109" activeCellId="0" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11555,6 +11680,1992 @@
         <v>0</v>
       </c>
     </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L92" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T92" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V92" s="3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP92" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ92" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L93" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T93" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V93" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP93" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ93" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L94" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T94" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V94" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC94" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP94" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ94" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L95" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T95" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V95" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC95" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ95" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L96" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T96" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V96" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ96" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="n">
+        <v>682</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L97" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="X97" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC97" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ97" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="n">
+        <v>686</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J98" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="L98" s="1" t="n">
+        <v>250000000000</v>
+      </c>
+      <c r="M98" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N98" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="O98" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W98" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC98" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ98" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA98" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM98" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP98" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ98" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="L99" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X99" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP99" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ99" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K100" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L100" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="U100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y100" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z100" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC100" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ100" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K101" s="1" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="L101" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="U101" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC101" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ101" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="n">
+        <v>690</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L102" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="O102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R102" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="S102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE102" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ102" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K103" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L103" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S103" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="U103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z103" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC103" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP103" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ103" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K104" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L104" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S104" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X104" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP104" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ104" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L105" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T105" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC105" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ105" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K106" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L106" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S106" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T106" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U106" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V106" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W106" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X106" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y106" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Z106" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC106" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ106" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K107" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L107" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S107" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T107" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U107" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V107" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W107" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X107" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z107" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC107" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ107" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="n">
+        <v>694</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L108" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="V108" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC108" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ108" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K109" s="1" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L109" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S109" s="5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U109" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W109" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X109" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z109" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC109" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP109" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ109" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
More updates and changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -962,7 +962,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -983,12 +983,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -1034,7 +1028,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1048,14 +1042,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1253,8 +1239,8 @@
   </sheetPr>
   <dimension ref="A1:BT109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K109" activeCellId="0" sqref="K109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L74" activeCellId="0" sqref="L74:O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9714,10 +9700,16 @@
         <v>5000</v>
       </c>
       <c r="L74" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M74" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N74" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O74" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q74" s="1" t="n">
         <v>0.35</v>
@@ -9821,10 +9813,16 @@
         <v>5000</v>
       </c>
       <c r="L75" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M75" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N75" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O75" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q75" s="1" t="n">
         <v>0.35</v>
@@ -9928,10 +9926,16 @@
         <v>5000</v>
       </c>
       <c r="L76" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M76" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N76" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O76" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q76" s="1" t="n">
         <v>0.35</v>
@@ -10035,10 +10039,16 @@
         <v>5000</v>
       </c>
       <c r="L77" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M77" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N77" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O77" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q77" s="1" t="n">
         <v>0.35</v>
@@ -10142,10 +10152,16 @@
         <v>5000</v>
       </c>
       <c r="L78" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M78" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N78" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O78" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q78" s="1" t="n">
         <v>0.35</v>
@@ -10249,10 +10265,16 @@
         <v>5000</v>
       </c>
       <c r="L79" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M79" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N79" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O79" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q79" s="1" t="n">
         <v>0.35</v>
@@ -10353,16 +10375,16 @@
         <v>1000000</v>
       </c>
       <c r="L80" s="1" t="n">
-        <v>250000000000</v>
+        <v>500000000000</v>
       </c>
       <c r="M80" s="1" t="n">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="N80" s="1" t="n">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="O80" s="1" t="n">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="W80" s="1" t="n">
         <v>0.6</v>
@@ -10463,10 +10485,16 @@
         <v>1000000</v>
       </c>
       <c r="L81" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M81" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N81" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O81" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q81" s="1" t="n">
         <v>0.3</v>
@@ -10570,10 +10598,16 @@
         <v>600000</v>
       </c>
       <c r="L82" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M82" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N82" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O82" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S82" s="1" t="n">
         <v>0.2</v>
@@ -10686,10 +10720,16 @@
         <v>1000000</v>
       </c>
       <c r="L83" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M83" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N83" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O83" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S83" s="1" t="n">
         <v>0.2</v>
@@ -10790,10 +10830,16 @@
         <v>5000</v>
       </c>
       <c r="L84" s="1" t="n">
-        <v>1000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M84" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N84" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O84" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q84" s="1" t="n">
         <v>0.85</v>
@@ -10900,10 +10946,16 @@
         <v>600000</v>
       </c>
       <c r="L85" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M85" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N85" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O85" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S85" s="1" t="n">
         <v>0.2</v>
@@ -11019,10 +11071,16 @@
         <v>600000</v>
       </c>
       <c r="L86" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M86" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N86" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O86" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S86" s="1" t="n">
         <v>0.2</v>
@@ -11135,10 +11193,16 @@
         <v>5000</v>
       </c>
       <c r="L87" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M87" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N87" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O87" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q87" s="1" t="n">
         <v>0.3</v>
@@ -11242,10 +11306,16 @@
         <v>600000</v>
       </c>
       <c r="L88" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M88" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N88" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O88" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S88" s="1" t="n">
         <v>0.2</v>
@@ -11361,10 +11431,16 @@
         <v>600000</v>
       </c>
       <c r="L89" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M89" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N89" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O89" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S89" s="1" t="n">
         <v>0.2</v>
@@ -11477,10 +11553,16 @@
         <v>5000</v>
       </c>
       <c r="L90" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M90" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N90" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O90" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="Q90" s="1" t="n">
         <v>0.3</v>
@@ -11584,10 +11666,16 @@
         <v>2000000</v>
       </c>
       <c r="L91" s="1" t="n">
-        <v>1000000000</v>
+        <v>500000000000</v>
+      </c>
+      <c r="M91" s="1" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N91" s="1" t="n">
+        <v>5000</v>
       </c>
       <c r="O91" s="1" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S91" s="1" t="n">
         <v>0.3</v>
@@ -11690,7 +11778,7 @@
       <c r="D92" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F92" s="4" t="s">
+      <c r="F92" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G92" s="2" t="s">
@@ -11797,7 +11885,7 @@
       <c r="D93" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F93" s="4" t="s">
+      <c r="F93" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G93" s="2" t="s">
@@ -11904,7 +11992,7 @@
       <c r="D94" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F94" s="4" t="s">
+      <c r="F94" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G94" s="2" t="s">
@@ -12011,7 +12099,7 @@
       <c r="D95" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F95" s="4" t="s">
+      <c r="F95" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G95" s="2" t="s">
@@ -12118,7 +12206,7 @@
       <c r="D96" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F96" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G96" s="2" t="s">
@@ -12225,7 +12313,7 @@
       <c r="D97" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="F97" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G97" s="2" t="s">
@@ -12329,7 +12417,7 @@
       <c r="D98" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F98" s="4" t="s">
+      <c r="F98" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G98" s="2" t="s">
@@ -12439,7 +12527,7 @@
       <c r="D99" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F99" s="4" t="s">
+      <c r="F99" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G99" s="2" t="s">
@@ -12543,7 +12631,7 @@
       <c r="D100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F100" s="4" t="s">
+      <c r="F100" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G100" s="2" t="s">
@@ -12662,7 +12750,7 @@
       <c r="D101" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F101" s="4" t="s">
+      <c r="F101" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G101" s="2" t="s">
@@ -12766,7 +12854,7 @@
       <c r="D102" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="F102" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G102" s="2" t="s">
@@ -12873,7 +12961,7 @@
       <c r="D103" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F103" s="4" t="s">
+      <c r="F103" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G103" s="2" t="s">
@@ -12992,7 +13080,7 @@
       <c r="D104" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F104" s="4" t="s">
+      <c r="F104" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G104" s="2" t="s">
@@ -13111,7 +13199,7 @@
       <c r="D105" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F105" s="4" t="s">
+      <c r="F105" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G105" s="2" t="s">
@@ -13126,7 +13214,7 @@
       <c r="O105" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" s="5" t="n">
+      <c r="Q105" s="3" t="n">
         <v>0.4</v>
       </c>
       <c r="T105" s="1" t="n">
@@ -13215,7 +13303,7 @@
       <c r="D106" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F106" s="4" t="s">
+      <c r="F106" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G106" s="2" t="s">
@@ -13334,7 +13422,7 @@
       <c r="D107" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="F107" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G107" s="2" t="s">
@@ -13453,7 +13541,7 @@
       <c r="D108" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="F108" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G108" s="2" t="s">
@@ -13468,7 +13556,7 @@
       <c r="O108" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" s="5" t="n">
+      <c r="Q108" s="3" t="n">
         <v>0.4</v>
       </c>
       <c r="V108" s="1" t="n">
@@ -13557,7 +13645,7 @@
       <c r="D109" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="F109" s="3" t="s">
         <v>275</v>
       </c>
       <c r="G109" s="2" t="s">
@@ -13575,7 +13663,7 @@
       <c r="O109" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="S109" s="5" t="n">
+      <c r="S109" s="3" t="n">
         <v>0.4</v>
       </c>
       <c r="T109" s="1" t="n">

</xml_diff>

<commit_message>
Minor fixes to holy items
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -1239,8 +1239,8 @@
   </sheetPr>
   <dimension ref="A1:BT109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S109" activeCellId="0" sqref="S109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BM18" activeCellId="0" sqref="BM18:BM109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3709,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="BM20" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN20" s="1" t="n">
         <v>0</v>
@@ -3816,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="BM21" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN21" s="1" t="n">
         <v>0</v>
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="BM22" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN22" s="1" t="n">
         <v>0</v>
@@ -4030,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="BM23" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN23" s="1" t="n">
         <v>0</v>
@@ -4137,7 +4137,7 @@
         <v>0</v>
       </c>
       <c r="BM24" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN24" s="1" t="n">
         <v>0</v>
@@ -4241,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="BM25" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN25" s="1" t="n">
         <v>0</v>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
       <c r="BM26" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN26" s="1" t="n">
         <v>0</v>
@@ -4452,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="BM27" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN27" s="1" t="n">
         <v>0</v>
@@ -4571,7 +4571,7 @@
         <v>0</v>
       </c>
       <c r="BM28" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN28" s="1" t="n">
         <v>0</v>
@@ -4675,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="BM29" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN29" s="1" t="n">
         <v>0</v>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="BM30" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN30" s="1" t="n">
         <v>0</v>
@@ -4901,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="BM31" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN31" s="1" t="n">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         <v>0</v>
       </c>
       <c r="BM32" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN32" s="1" t="n">
         <v>0</v>
@@ -5124,7 +5124,7 @@
         <v>0</v>
       </c>
       <c r="BM33" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN33" s="1" t="n">
         <v>0</v>
@@ -5243,7 +5243,7 @@
         <v>0</v>
       </c>
       <c r="BM34" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN34" s="1" t="n">
         <v>0</v>
@@ -5362,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="BM35" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN35" s="1" t="n">
         <v>0</v>
@@ -5466,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="BM36" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN36" s="1" t="n">
         <v>0</v>
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="BM37" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN37" s="1" t="n">
         <v>0</v>
@@ -7786,7 +7786,7 @@
         <v>0</v>
       </c>
       <c r="BM56" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN56" s="1" t="n">
         <v>0</v>
@@ -7893,7 +7893,7 @@
         <v>0</v>
       </c>
       <c r="BM57" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN57" s="1" t="n">
         <v>0</v>
@@ -8000,7 +8000,7 @@
         <v>0</v>
       </c>
       <c r="BM58" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN58" s="1" t="n">
         <v>0</v>
@@ -8107,7 +8107,7 @@
         <v>0</v>
       </c>
       <c r="BM59" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN59" s="1" t="n">
         <v>0</v>
@@ -8214,7 +8214,7 @@
         <v>0</v>
       </c>
       <c r="BM60" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN60" s="1" t="n">
         <v>0</v>
@@ -8318,7 +8318,7 @@
         <v>0</v>
       </c>
       <c r="BM61" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN61" s="1" t="n">
         <v>0</v>
@@ -8532,7 +8532,7 @@
         <v>0</v>
       </c>
       <c r="BM63" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN63" s="1" t="n">
         <v>0</v>
@@ -8651,7 +8651,7 @@
         <v>0</v>
       </c>
       <c r="BM64" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN64" s="1" t="n">
         <v>0</v>
@@ -8755,7 +8755,7 @@
         <v>0</v>
       </c>
       <c r="BM65" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN65" s="1" t="n">
         <v>0</v>
@@ -8862,7 +8862,7 @@
         <v>0</v>
       </c>
       <c r="BM66" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN66" s="1" t="n">
         <v>0</v>
@@ -8981,7 +8981,7 @@
         <v>0</v>
       </c>
       <c r="BM67" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN67" s="1" t="n">
         <v>0</v>
@@ -9100,7 +9100,7 @@
         <v>0</v>
       </c>
       <c r="BM68" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN68" s="1" t="n">
         <v>0</v>
@@ -9204,7 +9204,7 @@
         <v>0</v>
       </c>
       <c r="BM69" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN69" s="1" t="n">
         <v>0</v>
@@ -9323,7 +9323,7 @@
         <v>0</v>
       </c>
       <c r="BM70" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN70" s="1" t="n">
         <v>0</v>
@@ -9442,7 +9442,7 @@
         <v>0</v>
       </c>
       <c r="BM71" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN71" s="1" t="n">
         <v>0</v>
@@ -9546,7 +9546,7 @@
         <v>0</v>
       </c>
       <c r="BM72" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN72" s="1" t="n">
         <v>0</v>
@@ -9665,7 +9665,7 @@
         <v>0</v>
       </c>
       <c r="BM73" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN73" s="1" t="n">
         <v>0</v>
@@ -9778,7 +9778,7 @@
         <v>0</v>
       </c>
       <c r="BM74" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN74" s="1" t="n">
         <v>0</v>
@@ -9891,7 +9891,7 @@
         <v>0</v>
       </c>
       <c r="BM75" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN75" s="1" t="n">
         <v>0</v>
@@ -10004,7 +10004,7 @@
         <v>0</v>
       </c>
       <c r="BM76" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN76" s="1" t="n">
         <v>0</v>
@@ -10117,7 +10117,7 @@
         <v>0</v>
       </c>
       <c r="BM77" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN77" s="1" t="n">
         <v>0</v>
@@ -10230,7 +10230,7 @@
         <v>0</v>
       </c>
       <c r="BM78" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN78" s="1" t="n">
         <v>0</v>
@@ -10340,7 +10340,7 @@
         <v>0</v>
       </c>
       <c r="BM79" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN79" s="1" t="n">
         <v>0</v>
@@ -10560,7 +10560,7 @@
         <v>0</v>
       </c>
       <c r="BM81" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN81" s="1" t="n">
         <v>0</v>
@@ -10685,7 +10685,7 @@
         <v>0</v>
       </c>
       <c r="BM82" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN82" s="1" t="n">
         <v>0</v>
@@ -10795,7 +10795,7 @@
         <v>0</v>
       </c>
       <c r="BM83" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN83" s="1" t="n">
         <v>0</v>
@@ -10908,7 +10908,7 @@
         <v>0</v>
       </c>
       <c r="BM84" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN84" s="1" t="n">
         <v>0</v>
@@ -11033,7 +11033,7 @@
         <v>0</v>
       </c>
       <c r="BM85" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN85" s="1" t="n">
         <v>0</v>
@@ -11158,7 +11158,7 @@
         <v>0</v>
       </c>
       <c r="BM86" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN86" s="1" t="n">
         <v>0</v>
@@ -11268,7 +11268,7 @@
         <v>0</v>
       </c>
       <c r="BM87" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN87" s="1" t="n">
         <v>0</v>
@@ -11393,7 +11393,7 @@
         <v>0</v>
       </c>
       <c r="BM88" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN88" s="1" t="n">
         <v>0</v>
@@ -11518,7 +11518,7 @@
         <v>0</v>
       </c>
       <c r="BM89" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN89" s="1" t="n">
         <v>0</v>
@@ -11628,7 +11628,7 @@
         <v>0</v>
       </c>
       <c r="BM90" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN90" s="1" t="n">
         <v>0</v>
@@ -11753,7 +11753,7 @@
         <v>0</v>
       </c>
       <c r="BM91" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN91" s="1" t="n">
         <v>0</v>
@@ -11860,7 +11860,7 @@
         <v>0</v>
       </c>
       <c r="BM92" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN92" s="1" t="n">
         <v>0</v>
@@ -11967,7 +11967,7 @@
         <v>0</v>
       </c>
       <c r="BM93" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN93" s="1" t="n">
         <v>0</v>
@@ -12074,7 +12074,7 @@
         <v>0</v>
       </c>
       <c r="BM94" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN94" s="1" t="n">
         <v>0</v>
@@ -12181,7 +12181,7 @@
         <v>0</v>
       </c>
       <c r="BM95" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN95" s="1" t="n">
         <v>0</v>
@@ -12288,7 +12288,7 @@
         <v>0</v>
       </c>
       <c r="BM96" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN96" s="1" t="n">
         <v>0</v>
@@ -12392,7 +12392,7 @@
         <v>0</v>
       </c>
       <c r="BM97" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN97" s="1" t="n">
         <v>0</v>
@@ -12606,7 +12606,7 @@
         <v>0</v>
       </c>
       <c r="BM99" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN99" s="1" t="n">
         <v>0</v>
@@ -12725,7 +12725,7 @@
         <v>0</v>
       </c>
       <c r="BM100" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN100" s="1" t="n">
         <v>0</v>
@@ -12829,7 +12829,7 @@
         <v>0</v>
       </c>
       <c r="BM101" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN101" s="1" t="n">
         <v>0</v>
@@ -12936,7 +12936,7 @@
         <v>0</v>
       </c>
       <c r="BM102" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN102" s="1" t="n">
         <v>0</v>
@@ -13055,7 +13055,7 @@
         <v>0</v>
       </c>
       <c r="BM103" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN103" s="1" t="n">
         <v>0</v>
@@ -13174,7 +13174,7 @@
         <v>0</v>
       </c>
       <c r="BM104" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN104" s="1" t="n">
         <v>0</v>
@@ -13278,7 +13278,7 @@
         <v>0</v>
       </c>
       <c r="BM105" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN105" s="1" t="n">
         <v>0</v>
@@ -13397,7 +13397,7 @@
         <v>0</v>
       </c>
       <c r="BM106" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN106" s="1" t="n">
         <v>0</v>
@@ -13516,7 +13516,7 @@
         <v>0</v>
       </c>
       <c r="BM107" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN107" s="1" t="n">
         <v>0</v>
@@ -13620,7 +13620,7 @@
         <v>0</v>
       </c>
       <c r="BM108" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN108" s="1" t="n">
         <v>0</v>
@@ -13739,7 +13739,7 @@
         <v>0</v>
       </c>
       <c r="BM109" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BN109" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Various changes for the new quest line to get Faithless plate.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="348">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -953,6 +953,117 @@
   </si>
   <si>
     <t xml:space="preserve">A set of plate male that is crafted with the delusions of a broken man.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless Daggers of The Maiden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless Plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A maiden with no faith carried these daggers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless plate covered pistol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A gun plated in the faithless tears of yesterday.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless painted fan of time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fan painted with images of faithless people being murdered for their lack of belief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless priests mace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A priest once lost his faith in the one true God, this is the mace he was killed with.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless sand worms awl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand worms have no faith, they have no mind, they have nothing but hunger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mages Faithless stave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A stave created by a mage with no faith in hem self, her self or any one else that might have once existed in a realm of faithless memories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bring faith to those of the faithless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A spell that will bring faith to those with no faith, healing the mind and the wounds of yesterday,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strip those of their faith in the hell fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A spell to strip the faith from those who have their faith renewed by prayer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless plate sleeves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plate sleeves that slowly leach the faith of those who ware them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plate Shield of the faithless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A plate shield that indicates you have no faith, not even in the one true god.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy ring of faithless church</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a church lost to the time of sand, one that had no faith, one that was struck down.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guilded plate leggings of faithless children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple guilded plate leggings made by children with no faith.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow helmet of the leather plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A helmet created in the shadows of pain, one lost to the memories of yesterday.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless Hammer of dragons eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A hammer crafted of a stone dragons eye, alas even the dragon had no faith and hence his death was swift.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless plate gloves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloves that are simple, plated and offer protection but alas those who ware them have no faith.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boots of the faithless ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The ground you walk on is soiled by the blood of those with no faith.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bow of the witch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bow crafted by a witch who practices the magic of heretical love, alas her faith was stripped away from her.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faithless Plate of The Child</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A simple body of plate that a soldier wares. Crafted by a child who’s own tears were beaten out of his faithless body.</t>
   </si>
 </sst>
 </file>
@@ -1237,10 +1348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT109"/>
+  <dimension ref="A1:BT127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BM18" activeCellId="0" sqref="BM18:BM109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G130" activeCellId="0" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13754,6 +13865,1992 @@
         <v>0</v>
       </c>
     </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L110" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T110" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V110" s="3" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC110" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM110" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP110" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ110" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L111" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T111" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V111" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC111" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM111" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP111" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ111" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L112" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T112" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V112" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC112" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM112" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP112" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ112" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L113" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T113" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V113" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC113" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM113" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP113" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ113" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L114" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T114" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V114" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM114" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ114" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="n">
+        <v>682</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L115" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="X115" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC115" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM115" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP115" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ115" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="n">
+        <v>686</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="J116" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="L116" s="1" t="n">
+        <v>250000000000</v>
+      </c>
+      <c r="M116" s="1" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N116" s="1" t="n">
+        <v>2500</v>
+      </c>
+      <c r="O116" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="W116" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Y116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z116" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC116" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ116" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA116" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM116" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP116" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ116" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="L117" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q117" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X117" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z117" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC117" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM117" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP117" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ117" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K118" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L118" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S118" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="U118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y118" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z118" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC118" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM118" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP118" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ118" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="K119" s="1" t="n">
+        <v>1500000</v>
+      </c>
+      <c r="L119" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S119" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U119" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="Y119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM119" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP119" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ119" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="n">
+        <v>690</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L120" s="1" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="O120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R120" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="S120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM120" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP120" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ120" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K121" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L121" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="U121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z121" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC121" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM121" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ121" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K122" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L122" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="V122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="X122" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC122" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM122" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP122" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ122" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="n">
+        <v>691</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L123" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T123" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC123" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM123" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP123" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ123" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K124" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L124" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S124" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T124" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U124" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V124" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W124" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="X124" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y124" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Z124" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC124" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM124" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP124" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ124" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="n">
+        <v>427</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F125" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K125" s="1" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="L125" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="T125" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="U125" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="V125" s="1" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="W125" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="X125" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y125" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z125" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC125" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM125" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP125" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ125" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="n">
+        <v>694</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L126" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="V126" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC126" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM126" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP126" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ126" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K127" s="1" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="L127" s="1" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="O127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" s="3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="T127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U127" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="V127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="W127" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X127" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z127" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM127" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP127" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ127" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Cleaning up value objects to be enums and getting the swap items command into place
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/specialty-shops.xlsx
+++ b/resources/data-imports/Items/specialty-shops.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="363">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1064,6 +1064,51 @@
   </si>
   <si>
     <t xml:space="preserve">A simple body of plate that a soldier wares. Crafted by a child who’s own tears were beaten out of his faithless body.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infernal Thorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forged in the fires of the abyss, this dagger sears the soul of its victims.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackwater Shiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A deadly blade carried by the infamous Pirate Lords, swift and merciless.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soulpiercer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enchanted with spectral chains, this dagger binds the souls of the fallen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frostbite Fang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shard of frozen corruption, it freezes the hearts of those it cuts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stonefang Dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formed from the depths of the shifting earth, it trembles with untamed power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phantom's Veil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A blade of shimmering deception, warping reality with each strike.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oathsever Blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once wielded by fallen knights, this dagger carries the weight of broken oaths.</t>
   </si>
 </sst>
 </file>
@@ -1348,10 +1393,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT127"/>
+  <dimension ref="A1:BT134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G130" activeCellId="0" sqref="G130"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A134" activeCellId="0" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14293,7 +14338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
         <v>679</v>
       </c>
@@ -15848,6 +15893,963 @@
         <v>0</v>
       </c>
       <c r="BQ127" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E128" s="0"/>
+      <c r="F128" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G128" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="H128" s="0"/>
+      <c r="I128" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J128" s="0"/>
+      <c r="K128" s="0"/>
+      <c r="L128" s="0" t="n">
+        <v>150000000000</v>
+      </c>
+      <c r="M128" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N128" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P128" s="0"/>
+      <c r="Q128" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R128" s="0"/>
+      <c r="S128" s="0"/>
+      <c r="T128" s="0"/>
+      <c r="U128" s="0"/>
+      <c r="V128" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="W128" s="0"/>
+      <c r="X128" s="0"/>
+      <c r="Y128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA128" s="0"/>
+      <c r="AB128" s="0"/>
+      <c r="AC128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD128" s="0"/>
+      <c r="AE128" s="0"/>
+      <c r="AF128" s="0"/>
+      <c r="AG128" s="0"/>
+      <c r="AH128" s="0"/>
+      <c r="AI128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN128" s="0"/>
+      <c r="AO128" s="0"/>
+      <c r="AP128" s="0"/>
+      <c r="AQ128" s="0"/>
+      <c r="AR128" s="0"/>
+      <c r="AS128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT128" s="0"/>
+      <c r="AU128" s="0"/>
+      <c r="AV128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW128" s="0"/>
+      <c r="AX128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ128" s="0"/>
+      <c r="BA128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH128" s="0"/>
+      <c r="BI128" s="0"/>
+      <c r="BJ128" s="0"/>
+      <c r="BK128" s="0"/>
+      <c r="BL128" s="0"/>
+      <c r="BM128" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ128" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E129" s="0"/>
+      <c r="F129" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G129" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="H129" s="0"/>
+      <c r="I129" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J129" s="0"/>
+      <c r="K129" s="0"/>
+      <c r="L129" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="M129" s="0"/>
+      <c r="N129" s="0"/>
+      <c r="O129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="0"/>
+      <c r="Q129" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R129" s="0"/>
+      <c r="S129" s="0"/>
+      <c r="T129" s="0"/>
+      <c r="U129" s="0"/>
+      <c r="V129" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="W129" s="0"/>
+      <c r="X129" s="0"/>
+      <c r="Y129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA129" s="0"/>
+      <c r="AB129" s="0"/>
+      <c r="AC129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD129" s="0"/>
+      <c r="AE129" s="0"/>
+      <c r="AF129" s="0"/>
+      <c r="AG129" s="0"/>
+      <c r="AH129" s="0"/>
+      <c r="AI129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN129" s="0"/>
+      <c r="AO129" s="0"/>
+      <c r="AP129" s="0"/>
+      <c r="AQ129" s="0"/>
+      <c r="AR129" s="0"/>
+      <c r="AS129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT129" s="0"/>
+      <c r="AU129" s="0"/>
+      <c r="AV129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW129" s="0"/>
+      <c r="AX129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ129" s="0"/>
+      <c r="BA129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH129" s="0"/>
+      <c r="BI129" s="0"/>
+      <c r="BJ129" s="0"/>
+      <c r="BK129" s="0"/>
+      <c r="BL129" s="0"/>
+      <c r="BM129" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ129" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E130" s="0"/>
+      <c r="F130" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G130" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="H130" s="0"/>
+      <c r="I130" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="J130" s="0"/>
+      <c r="K130" s="0"/>
+      <c r="L130" s="0" t="n">
+        <v>250000000000</v>
+      </c>
+      <c r="M130" s="0" t="n">
+        <v>25000</v>
+      </c>
+      <c r="N130" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="O130" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P130" s="0"/>
+      <c r="Q130" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="R130" s="0"/>
+      <c r="S130" s="0"/>
+      <c r="T130" s="0"/>
+      <c r="U130" s="0"/>
+      <c r="V130" s="0" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="W130" s="0"/>
+      <c r="X130" s="0"/>
+      <c r="Y130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA130" s="0"/>
+      <c r="AB130" s="0"/>
+      <c r="AC130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD130" s="0"/>
+      <c r="AE130" s="0"/>
+      <c r="AF130" s="0"/>
+      <c r="AG130" s="0"/>
+      <c r="AH130" s="0"/>
+      <c r="AI130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN130" s="0"/>
+      <c r="AO130" s="0"/>
+      <c r="AP130" s="0"/>
+      <c r="AQ130" s="0"/>
+      <c r="AR130" s="0"/>
+      <c r="AS130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT130" s="0"/>
+      <c r="AU130" s="0"/>
+      <c r="AV130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW130" s="0"/>
+      <c r="AX130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ130" s="0"/>
+      <c r="BA130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH130" s="0"/>
+      <c r="BI130" s="0"/>
+      <c r="BJ130" s="0"/>
+      <c r="BK130" s="0"/>
+      <c r="BL130" s="0"/>
+      <c r="BM130" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ130" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E131" s="0"/>
+      <c r="F131" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G131" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="H131" s="0"/>
+      <c r="I131" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J131" s="0"/>
+      <c r="K131" s="0"/>
+      <c r="L131" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="M131" s="0"/>
+      <c r="N131" s="0"/>
+      <c r="O131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" s="0"/>
+      <c r="Q131" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R131" s="0"/>
+      <c r="S131" s="0"/>
+      <c r="T131" s="0"/>
+      <c r="U131" s="0"/>
+      <c r="V131" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="W131" s="0"/>
+      <c r="X131" s="0"/>
+      <c r="Y131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA131" s="0"/>
+      <c r="AB131" s="0"/>
+      <c r="AC131" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD131" s="0"/>
+      <c r="AE131" s="0"/>
+      <c r="AF131" s="0"/>
+      <c r="AG131" s="0"/>
+      <c r="AH131" s="0"/>
+      <c r="AI131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN131" s="0"/>
+      <c r="AO131" s="0"/>
+      <c r="AP131" s="0"/>
+      <c r="AQ131" s="0"/>
+      <c r="AR131" s="0"/>
+      <c r="AS131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT131" s="0"/>
+      <c r="AU131" s="0"/>
+      <c r="AV131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW131" s="0"/>
+      <c r="AX131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ131" s="0"/>
+      <c r="BA131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH131" s="0"/>
+      <c r="BI131" s="0"/>
+      <c r="BJ131" s="0"/>
+      <c r="BK131" s="0"/>
+      <c r="BL131" s="0"/>
+      <c r="BM131" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ131" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E132" s="0"/>
+      <c r="F132" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="G132" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="H132" s="0"/>
+      <c r="I132" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="J132" s="0"/>
+      <c r="K132" s="0"/>
+      <c r="L132" s="0" t="n">
+        <v>500000000000</v>
+      </c>
+      <c r="M132" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="N132" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="O132" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P132" s="0"/>
+      <c r="Q132" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="R132" s="0"/>
+      <c r="S132" s="0"/>
+      <c r="T132" s="0"/>
+      <c r="U132" s="0"/>
+      <c r="V132" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="W132" s="0"/>
+      <c r="X132" s="0"/>
+      <c r="Y132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA132" s="0"/>
+      <c r="AB132" s="0"/>
+      <c r="AC132" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD132" s="0"/>
+      <c r="AE132" s="0"/>
+      <c r="AF132" s="0"/>
+      <c r="AG132" s="0"/>
+      <c r="AH132" s="0"/>
+      <c r="AI132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN132" s="0"/>
+      <c r="AO132" s="0"/>
+      <c r="AP132" s="0"/>
+      <c r="AQ132" s="0"/>
+      <c r="AR132" s="0"/>
+      <c r="AS132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT132" s="0"/>
+      <c r="AU132" s="0"/>
+      <c r="AV132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW132" s="0"/>
+      <c r="AX132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ132" s="0"/>
+      <c r="BA132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH132" s="0"/>
+      <c r="BI132" s="0"/>
+      <c r="BJ132" s="0"/>
+      <c r="BK132" s="0"/>
+      <c r="BL132" s="0"/>
+      <c r="BM132" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ132" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E133" s="0"/>
+      <c r="F133" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G133" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="H133" s="0"/>
+      <c r="I133" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J133" s="0"/>
+      <c r="K133" s="0"/>
+      <c r="L133" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="M133" s="0"/>
+      <c r="N133" s="0"/>
+      <c r="O133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" s="0"/>
+      <c r="Q133" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="R133" s="0"/>
+      <c r="S133" s="0"/>
+      <c r="T133" s="0"/>
+      <c r="U133" s="0"/>
+      <c r="V133" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W133" s="0"/>
+      <c r="X133" s="0"/>
+      <c r="Y133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA133" s="0"/>
+      <c r="AB133" s="0"/>
+      <c r="AC133" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD133" s="0"/>
+      <c r="AE133" s="0"/>
+      <c r="AF133" s="0"/>
+      <c r="AG133" s="0"/>
+      <c r="AH133" s="0"/>
+      <c r="AI133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN133" s="0"/>
+      <c r="AO133" s="0"/>
+      <c r="AP133" s="0"/>
+      <c r="AQ133" s="0"/>
+      <c r="AR133" s="0"/>
+      <c r="AS133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT133" s="0"/>
+      <c r="AU133" s="0"/>
+      <c r="AV133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW133" s="0"/>
+      <c r="AX133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ133" s="0"/>
+      <c r="BA133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH133" s="0"/>
+      <c r="BI133" s="0"/>
+      <c r="BJ133" s="0"/>
+      <c r="BK133" s="0"/>
+      <c r="BL133" s="0"/>
+      <c r="BM133" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ133" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E134" s="0"/>
+      <c r="F134" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="G134" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="H134" s="0"/>
+      <c r="I134" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J134" s="0"/>
+      <c r="K134" s="0"/>
+      <c r="L134" s="0" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="M134" s="0"/>
+      <c r="N134" s="0"/>
+      <c r="O134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P134" s="0"/>
+      <c r="Q134" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="R134" s="0"/>
+      <c r="S134" s="0"/>
+      <c r="T134" s="0"/>
+      <c r="U134" s="0"/>
+      <c r="V134" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="W134" s="0"/>
+      <c r="X134" s="0"/>
+      <c r="Y134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA134" s="0"/>
+      <c r="AB134" s="0"/>
+      <c r="AC134" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD134" s="0"/>
+      <c r="AE134" s="0"/>
+      <c r="AF134" s="0"/>
+      <c r="AG134" s="0"/>
+      <c r="AH134" s="0"/>
+      <c r="AI134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN134" s="0"/>
+      <c r="AO134" s="0"/>
+      <c r="AP134" s="0"/>
+      <c r="AQ134" s="0"/>
+      <c r="AR134" s="0"/>
+      <c r="AS134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT134" s="0"/>
+      <c r="AU134" s="0"/>
+      <c r="AV134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW134" s="0"/>
+      <c r="AX134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ134" s="0"/>
+      <c r="BA134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH134" s="0"/>
+      <c r="BI134" s="0"/>
+      <c r="BJ134" s="0"/>
+      <c r="BK134" s="0"/>
+      <c r="BL134" s="0"/>
+      <c r="BM134" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="BN134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ134" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>